<commit_message>
added doc until motif analysis
</commit_message>
<xml_diff>
--- a/docs/summary_data.xlsx
+++ b/docs/summary_data.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jihedchouaref/Dropbox/Work/atac_veronica/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jihedchouaref/Dropbox/Work/ATAC-seq/atac_veronica/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CB1BD4-2B37-C846-B852-C4FDB5C9A835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A368681-9E3E-C445-BCFC-AE96E20B486A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{9E7B3717-0523-D140-8FDB-8154D4C28D11}"/>
+    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{9E7B3717-0523-D140-8FDB-8154D4C28D11}"/>
   </bookViews>
   <sheets>
     <sheet name="setup" sheetId="1" r:id="rId1"/>
-    <sheet name="peals" sheetId="2" r:id="rId2"/>
+    <sheet name="peaks" sheetId="2" r:id="rId2"/>
     <sheet name="differential peaks" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -587,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C225AD4-07A5-E14E-A73F-1C895E2686A0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -634,7 +634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1641CAF-BEAC-A94D-8800-98EFCD2D9AAA}">
   <dimension ref="A2:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
first addition of December  analysis
</commit_message>
<xml_diff>
--- a/docs/summary_data.xlsx
+++ b/docs/summary_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jihedchouaref/Dropbox/Work/ATAC-seq/atac_veronica/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A368681-9E3E-C445-BCFC-AE96E20B486A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B98DABF-9B66-E54F-845A-1C76F619FC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{9E7B3717-0523-D140-8FDB-8154D4C28D11}"/>
+    <workbookView xWindow="2740" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{9E7B3717-0523-D140-8FDB-8154D4C28D11}"/>
   </bookViews>
   <sheets>
     <sheet name="setup" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>WT1</t>
   </si>
@@ -90,6 +90,33 @@
   </si>
   <si>
     <t>More accessible in KO</t>
+  </si>
+  <si>
+    <t>July 2021</t>
+  </si>
+  <si>
+    <t>KODec</t>
+  </si>
+  <si>
+    <t>WTDec</t>
+  </si>
+  <si>
+    <t>KOJul1</t>
+  </si>
+  <si>
+    <t>KOJul2</t>
+  </si>
+  <si>
+    <t>Dec 2021</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>without sexs chromosome</t>
+  </si>
+  <si>
+    <t>Diffbind Dec 2021</t>
   </si>
 </sst>
 </file>
@@ -111,15 +138,27 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -142,14 +181,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -585,81 +645,184 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C225AD4-07A5-E14E-A73F-1C895E2686A0}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>28992</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>28288</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>24902</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3">
+        <v>24217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
         <v>37473</v>
       </c>
+      <c r="C4" s="5"/>
+      <c r="D4">
+        <v>36436</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3">
+        <v>46140</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5">
+        <v>44699</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4">
+        <v>76930</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6">
+        <v>74870</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4">
+        <v>45832</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7">
+        <v>44578</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="4">
+        <v>49211</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8">
+        <v>47935</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C5:C8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1641CAF-BEAC-A94D-8800-98EFCD2D9AAA}">
-  <dimension ref="A2:B3"/>
+  <dimension ref="A2:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="1">
         <v>2046</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="1">
         <v>269</v>
       </c>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1">
+        <v>103</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1">
+        <v>194</v>
+      </c>
+      <c r="C7" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C6:C7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added motif analysis diffbind
</commit_message>
<xml_diff>
--- a/docs/summary_data.xlsx
+++ b/docs/summary_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jihedchouaref/Dropbox/Work/ATAC-seq/atac_veronica/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B98DABF-9B66-E54F-845A-1C76F619FC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E785F925-ED0B-9349-B7C3-A27AC5FC45DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2740" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{9E7B3717-0523-D140-8FDB-8154D4C28D11}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>WT1</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>Diffbind Dec 2021</t>
+  </si>
+  <si>
+    <t>Homer all peaks</t>
+  </si>
+  <si>
+    <t>Homer consistent</t>
   </si>
 </sst>
 </file>
@@ -766,10 +772,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1641CAF-BEAC-A94D-8800-98EFCD2D9AAA}">
-  <dimension ref="A2:C7"/>
+  <dimension ref="A2:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -818,10 +824,52 @@
       </c>
       <c r="C7" s="6"/>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1658</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1879</v>
+      </c>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>36</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1">
+        <v>209</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C14:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added the analysis excluding DecKO1
</commit_message>
<xml_diff>
--- a/docs/summary_data.xlsx
+++ b/docs/summary_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jihedchouaref/Dropbox/Work/ATAC-seq/atac_veronica/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E785F925-ED0B-9349-B7C3-A27AC5FC45DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AC7F26-6728-5346-80DB-66D71C7125D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{9E7B3717-0523-D140-8FDB-8154D4C28D11}"/>
+    <workbookView xWindow="2720" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{9E7B3717-0523-D140-8FDB-8154D4C28D11}"/>
   </bookViews>
   <sheets>
     <sheet name="setup" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>WT1</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Homer consistent</t>
+  </si>
+  <si>
+    <t>Homer excluding DecKO1</t>
   </si>
 </sst>
 </file>
@@ -200,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -218,6 +221,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,16 +776,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1641CAF-BEAC-A94D-8800-98EFCD2D9AAA}">
-  <dimension ref="A2:C15"/>
+  <dimension ref="A2:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A18" sqref="A18:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -864,12 +868,33 @@
       </c>
       <c r="C15" s="6"/>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1725</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="7">
+        <v>1371</v>
+      </c>
+      <c r="C19" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C18:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>